<commit_message>
error when loading map
</commit_message>
<xml_diff>
--- a/battles/Erigon/Erigon.xlsx
+++ b/battles/Erigon/Erigon.xlsx
@@ -1,40 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\training\gboh-companion\battles\Erigon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FF7167-1424-465C-813B-947BE7927AF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macedonian" sheetId="1" r:id="rId1"/>
     <sheet name="Phocian" sheetId="2" r:id="rId2"/>
     <sheet name="Leaders" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId4"/>
-    <pivotCache cacheId="20" r:id="rId5"/>
-    <pivotCache cacheId="25" r:id="rId6"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>Kind</t>
   </si>
@@ -232,9 +239,6 @@
   </si>
   <si>
     <t>PLC</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>(vide)</t>
@@ -309,7 +313,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -465,90 +469,90 @@
     </xf>
   </cellXfs>
   <cellStyles count="85">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,7 +569,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Laurent Kloetzer" refreshedDate="44570.632029166663" createdVersion="6" refreshedVersion="4" minRefreshableVersion="3" recordCount="21">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent Kloetzer" refreshedDate="44570.632029166663" createdVersion="6" refreshedVersion="4" minRefreshableVersion="3" recordCount="21" xr:uid="{00000000-000A-0000-FFFF-FFFF11000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H20" sheet="Phocian"/>
   </cacheSource>
@@ -624,7 +628,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Laurent Kloetzer" refreshedDate="44570.632083796299" createdVersion="6" refreshedVersion="4" minRefreshableVersion="3" recordCount="21">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent Kloetzer" refreshedDate="44570.632083796299" createdVersion="6" refreshedVersion="4" minRefreshableVersion="3" recordCount="21" xr:uid="{00000000-000A-0000-FFFF-FFFF14000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N20" sheet="Phocian"/>
   </cacheSource>
@@ -686,7 +690,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Laurent Kloetzer" refreshedDate="44570.638975578702" createdVersion="6" refreshedVersion="4" minRefreshableVersion="3" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent Kloetzer" refreshedDate="44570.638975578702" createdVersion="6" refreshedVersion="4" minRefreshableVersion="3" recordCount="2" xr:uid="{00000000-000A-0000-FFFF-FFFF19000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:M3" sheet="Macedonian"/>
   </cacheSource>
@@ -1356,7 +1360,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A25:B29" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField axis="axisRow" showAll="0">
@@ -1431,7 +1435,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M25:N28" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -1488,7 +1492,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N25:O31" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -1553,7 +1557,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A25:B41" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1981,22 +1985,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" customWidth="1"/>
+    <col min="13" max="13" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2037,18 +2041,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2">
         <v>6</v>
@@ -2065,18 +2069,18 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3">
         <v>6</v>
@@ -2093,18 +2097,18 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -2121,18 +2125,18 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -2149,18 +2153,18 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -2177,7 +2181,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2185,7 +2189,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2208,7 +2212,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2216,7 +2220,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -2239,12 +2243,12 @@
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2270,12 +2274,12 @@
         <v>750</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -2301,18 +2305,18 @@
         <v>750</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -2332,18 +2336,18 @@
         <v>750</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -2363,18 +2367,18 @@
         <v>750</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -2394,18 +2398,18 @@
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -2425,18 +2429,18 @@
         <v>750</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -2445,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="7"/>
@@ -2456,18 +2460,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -2476,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="7"/>
@@ -2487,18 +2491,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17">
         <v>7</v>
@@ -2515,7 +2519,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2532,7 +2536,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2540,7 +2544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
@@ -2568,7 +2572,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>6</v>
       </c>
@@ -2582,7 +2586,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
@@ -2603,22 +2607,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" customWidth="1"/>
+    <col min="14" max="14" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2662,7 +2666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2694,7 +2698,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +2730,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2758,7 +2762,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2790,7 +2794,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2843,7 +2847,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="4"/>
@@ -2854,7 +2858,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2950,7 +2954,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2981,7 +2985,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3043,7 +3047,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -3105,7 +3109,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -3137,7 +3141,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -3169,7 +3173,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -3201,7 +3205,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -3230,7 +3234,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -3258,7 +3262,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3275,7 +3279,7 @@
         <v>14750</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -3283,7 +3287,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -3297,7 +3301,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
@@ -3311,7 +3315,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>5</v>
       </c>
@@ -3325,7 +3329,7 @@
         <v>14250</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -3339,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>6</v>
       </c>
@@ -3353,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>7</v>
       </c>
@@ -3367,7 +3371,7 @@
         <v>14750</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
@@ -3375,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>5</v>
       </c>
@@ -3383,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -3391,7 +3395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>5</v>
       </c>
@@ -3399,7 +3403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>6</v>
       </c>
@@ -3407,7 +3411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>51</v>
       </c>
@@ -3415,7 +3419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>5</v>
       </c>
@@ -3423,19 +3427,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>24</v>
       </c>
@@ -3456,16 +3460,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3505,7 +3509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3525,12 +3529,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -3545,12 +3549,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>6</v>

</xml_diff>